<commit_message>
Updated the ExcelWriter.java file
</commit_message>
<xml_diff>
--- a/test-files/old/Room Information (Responses).xlsx
+++ b/test-files/old/Room Information (Responses).xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\workspace\523-Music-Scheduler\test-files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="8140"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Timestamp</t>
   </si>
@@ -91,13 +91,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -125,8 +137,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -134,7 +148,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -193,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,7 +244,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,23 +429,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
-    <col min="5" max="8" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" customWidth="1"/>
+    <col min="5" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="1">
         <v>42070.599055081024</v>
       </c>
@@ -481,7 +497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="1">
         <v>42070.599336550928</v>
       </c>
@@ -504,15 +520,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>42070.599336550928</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
@@ -521,33 +540,16 @@
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>42070.599336550928</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>